<commit_message>
BOM and Testing procedure added
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>SL.NO</t>
   </si>
@@ -67,13 +67,16 @@
   </si>
   <si>
     <t>Datasheet</t>
+  </si>
+  <si>
+    <t>BOM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,6 +90,14 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -128,7 +139,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -138,6 +149,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -433,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -448,63 +460,54 @@
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" s="1" customFormat="1">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="1:5">
+      <c r="C1" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1"/>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="2">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>5</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C4" s="3"/>
       <c r="D4" s="2">
         <v>1</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
@@ -514,28 +517,28 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>9</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C6" s="3"/>
       <c r="D6" s="2">
         <v>1</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
@@ -544,29 +547,45 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="2">
-        <v>1</v>
-      </c>
-      <c r="E8" s="4" t="s">
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1"/>
-    <hyperlink ref="E4" r:id="rId2"/>
-    <hyperlink ref="E8" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E4" r:id="rId1"/>
+    <hyperlink ref="E5" r:id="rId2"/>
+    <hyperlink ref="E9" r:id="rId3"/>
+    <hyperlink ref="E6" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>